<commit_message>
gw: update tas village list
</commit_message>
<xml_diff>
--- a/LF/TAS/Guinee Bissau/gw_lf_tas1_2_partcipants_202206.xlsx
+++ b/LF/TAS/Guinee Bissau/gw_lf_tas1_2_partcipants_202206.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -258,10 +258,10 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>(Jun 2022) 5. TAS1 FL - Formulário de participantes V2</t>
-  </si>
-  <si>
-    <t>gw_lf_tas1_2_partcipants_202206_v2</t>
+    <t>(Jun 2022) 5. TAS1 FL - Formulário de participantes V2.1</t>
+  </si>
+  <si>
+    <t>gw_lf_tas1_2_partcipants_202206_v2_1</t>
   </si>
   <si>
     <t>Portuguese</t>
@@ -273,9 +273,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -329,9 +329,69 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -343,6 +403,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -352,34 +449,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -394,82 +470,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -486,19 +486,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -510,67 +636,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -582,91 +648,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -725,6 +725,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -744,22 +774,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -768,7 +783,16 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -788,21 +812,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -813,157 +822,148 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1361,7 +1361,7 @@
   <sheetPr/>
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -1928,8 +1928,8 @@
   <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>

</xml_diff>

<commit_message>
gw: tas1 update location list
</commit_message>
<xml_diff>
--- a/LF/TAS/Guinee Bissau/gw_lf_tas1_2_partcipants_202206.xlsx
+++ b/LF/TAS/Guinee Bissau/gw_lf_tas1_2_partcipants_202206.xlsx
@@ -258,10 +258,10 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>(Jun 2022) 5. TAS1 FL - Formulário de participantes (Phase 2)</t>
-  </si>
-  <si>
-    <t>gw_lf_tas1_2_partcipants_phase2_202206</t>
+    <t>(Jun 2022) 5. TAS1 FL - Formulário de participantes (Phase 2) V2</t>
+  </si>
+  <si>
+    <t>gw_lf_tas1_2_partcipants_phase2_202206_v2</t>
   </si>
   <si>
     <t>Portuguese</t>
@@ -272,10 +272,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -320,6 +320,74 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -329,24 +397,24 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -358,38 +426,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -410,52 +456,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -465,7 +465,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -486,6 +486,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -498,61 +510,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -564,90 +654,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -655,18 +667,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -725,11 +725,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -738,7 +744,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -759,21 +765,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -788,25 +779,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -822,151 +804,169 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1929,12 +1929,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="49.6222222222222" customWidth="1"/>
+    <col min="1" max="1" width="54.1111111111111" customWidth="1"/>
     <col min="2" max="2" width="43.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>